<commit_message>
Full Fourth step Completed
</commit_message>
<xml_diff>
--- a/files/merge_converter.xlsx
+++ b/files/merge_converter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>one</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>five_percentage_difference_a</t>
+  </si>
+  <si>
+    <t>pec_two</t>
+  </si>
+  <si>
+    <t>pec_five</t>
   </si>
 </sst>
 </file>
@@ -417,13 +423,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N660"/>
+  <dimension ref="A1:P660"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +472,14 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="2">
         <v>44272.40055555557</v>
       </c>
@@ -492,8 +504,14 @@
       <c r="J2">
         <v>0.1519753524513725</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2">
+        <v>0.004846134448298317</v>
+      </c>
+      <c r="P2">
+        <v>0.006656051969724575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="2">
         <v>44272.4005787037</v>
       </c>
@@ -530,8 +548,14 @@
       <c r="N3">
         <v>2.400457251372501E-05</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3">
+        <v>42.13228922028998</v>
+      </c>
+      <c r="P3">
+        <v>57.86771077971002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="2">
         <v>44272.400625</v>
       </c>
@@ -563,7 +587,7 @@
         <v>6.546701594667415E-06</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" s="2">
         <v>44272.40063657407</v>
       </c>
@@ -595,7 +619,7 @@
         <v>-2.466947189441737E-05</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6" s="2">
         <v>44272.40065972223</v>
       </c>
@@ -633,7 +657,7 @@
         <v>6.103435340854002E-06</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" s="2">
         <v>44272.40070601852</v>
       </c>
@@ -671,7 +695,7 @@
         <v>4.954352821368024E-05</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="A8" s="2">
         <v>44272.40071759259</v>
       </c>
@@ -703,7 +727,7 @@
         <v>-6.648993806923631E-07</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:16">
       <c r="A9" s="2">
         <v>44272.40074074074</v>
       </c>
@@ -735,7 +759,7 @@
         <v>1.484941950244401E-05</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:16">
       <c r="A10" s="2">
         <v>44272.40075231482</v>
       </c>
@@ -767,7 +791,7 @@
         <v>-3.950184269482793E-05</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:16">
       <c r="A11" s="2">
         <v>44272.40079861111</v>
       </c>
@@ -805,7 +829,7 @@
         <v>1.723623779215089E-05</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:16">
       <c r="A12" s="2">
         <v>44272.40081018519</v>
       </c>
@@ -843,7 +867,7 @@
         <v>1.135443557823135E-05</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:16">
       <c r="A13" s="2">
         <v>44272.40086805557</v>
       </c>
@@ -881,7 +905,7 @@
         <v>4.800914502745002E-05</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:16">
       <c r="A14" s="2">
         <v>44272.4008912037</v>
       </c>
@@ -913,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:16">
       <c r="A15" s="2">
         <v>44272.40090277778</v>
       </c>
@@ -951,7 +975,7 @@
         <v>1.222391938376921E-05</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:16">
       <c r="A16" s="2">
         <v>44272.40092592594</v>
       </c>

</xml_diff>